<commit_message>
Ejercicio de Amazon terminado
</commit_message>
<xml_diff>
--- a/tests/data.xlsx
+++ b/tests/data.xlsx
@@ -1,55 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjfm/WebstormProjects/Framework-webdriver-video/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis Gerardo Olguin\Documents\Framework GlobalHitss\FrameworkInterno\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414A40CB-D26B-F34A-86DA-AF45E1711CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270E433E-02B6-4EC7-95EA-6F2BBD4DAF3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13140" yWindow="2292" windowWidth="9900" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>password</t>
+    <t>Baquetas</t>
   </si>
   <si>
-    <t>user</t>
+    <t>Nintendo Switch</t>
   </si>
   <si>
-    <t>username</t>
+    <t>Audifonos Inalambricos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -77,16 +64,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -99,9 +84,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -139,7 +124,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -245,7 +230,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -387,7 +372,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -395,35 +380,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>